<commit_message>
Deploy CIE IG to GitHub Pages
</commit_message>
<xml_diff>
--- a/StructureDefinition-CIEPatient.xlsx
+++ b/StructureDefinition-CIEPatient.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-09T09:25:32-04:00</t>
+    <t>2025-07-09T09:31:51-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -696,7 +696,7 @@
     <t>If the value is a full URI, then the system SHALL be urn:ietf:rfc:3986.  The value's primary purpose is computational mapping.  As a result, it may be normalized for comparison purposes (e.g. removing non-significant whitespace, dashes, etc.)  A value formatted for human display can be conveyed using the [Rendered Value extension](http://hl7.org/fhir/R4/extension-rendered-value.html). Identifier.value is to be treated as case sensitive unless knowledge of the Identifier.system allows the processer to be confident that non-case-sensitive processing is safe.</t>
   </si>
   <si>
-    <t>22990393</t>
+    <t>12345</t>
   </si>
   <si>
     <t>123456</t>

</xml_diff>